<commit_message>
add big data with max bundle size=2
</commit_message>
<xml_diff>
--- a/outputs-card-100-families-6-games.xlsx
+++ b/outputs-card-100-families-6-games.xlsx
@@ -12881,22 +12881,22 @@
         <v>29</v>
       </c>
       <c r="AI3" t="n">
-        <v>27</v>
+        <v>292</v>
       </c>
       <c r="AJ3" t="n">
-        <v>30</v>
+        <v>272</v>
       </c>
       <c r="AK3" t="n">
-        <v>29</v>
+        <v>294</v>
       </c>
       <c r="AL3" t="n">
-        <v>29</v>
+        <v>294</v>
       </c>
       <c r="AM3" t="n">
-        <v>33</v>
+        <v>262</v>
       </c>
       <c r="AN3" t="n">
-        <v>31</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4">
@@ -12996,22 +12996,22 @@
         <v>69</v>
       </c>
       <c r="AI4" t="n">
-        <v>83</v>
+        <v>740</v>
       </c>
       <c r="AJ4" t="n">
-        <v>76</v>
+        <v>871</v>
       </c>
       <c r="AK4" t="n">
-        <v>80</v>
+        <v>738</v>
       </c>
       <c r="AL4" t="n">
-        <v>71</v>
+        <v>735</v>
       </c>
       <c r="AM4" t="n">
-        <v>57</v>
+        <v>931</v>
       </c>
       <c r="AN4" t="n">
-        <v>70</v>
+        <v>672</v>
       </c>
     </row>
     <row r="6">
@@ -13111,22 +13111,22 @@
         <v>6</v>
       </c>
       <c r="AI6" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="AJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>87</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="n">
         <v>11</v>
       </c>
-      <c r="AK6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>15</v>
-      </c>
       <c r="AN6" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
@@ -13226,22 +13226,22 @@
         <v>10</v>
       </c>
       <c r="AI7" t="n">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="AJ7" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="AK7" t="n">
-        <v>12</v>
+        <v>103</v>
       </c>
       <c r="AL7" t="n">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="AM7" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AN7" t="n">
-        <v>12</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8">
@@ -13341,22 +13341,22 @@
         <v>10</v>
       </c>
       <c r="AI8" t="n">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="AJ8" t="n">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="AK8" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="AL8" t="n">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="AM8" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="AN8" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -13456,22 +13456,22 @@
         <v>2</v>
       </c>
       <c r="AI9" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="AJ9" t="n">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="AK9" t="n">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="AL9" t="n">
         <v>0</v>
       </c>
       <c r="AM9" t="n">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="AN9" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -13571,22 +13571,22 @@
         <v>1</v>
       </c>
       <c r="AI10" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AJ10" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AK10" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AL10" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AM10" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="AN10" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -13648,7 +13648,7 @@
         <v>29</v>
       </c>
       <c r="J14" t="n">
-        <v>30</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15">
@@ -13673,7 +13673,7 @@
         <v>74</v>
       </c>
       <c r="J15" t="n">
-        <v>73</v>
+        <v>781</v>
       </c>
     </row>
     <row r="16">
@@ -13698,7 +13698,7 @@
         <v>5</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -13723,7 +13723,7 @@
         <v>10</v>
       </c>
       <c r="J17" t="n">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18">
@@ -13748,7 +13748,7 @@
         <v>9</v>
       </c>
       <c r="J18" t="n">
-        <v>5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19">
@@ -13773,7 +13773,7 @@
         <v>4</v>
       </c>
       <c r="J19" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20">
@@ -13798,7 +13798,7 @@
         <v>2</v>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
@@ -13830,7 +13830,7 @@
         <v>29</v>
       </c>
       <c r="J23" t="n">
-        <v>41</v>
+        <v>282</v>
       </c>
     </row>
     <row r="24">
@@ -13855,7 +13855,7 @@
         <v>71</v>
       </c>
       <c r="J24" t="n">
-        <v>39</v>
+        <v>718</v>
       </c>
     </row>
     <row r="25">
@@ -13880,7 +13880,7 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -13987,7 +13987,7 @@
         <v>78</v>
       </c>
       <c r="J32" t="n">
-        <v>112</v>
+        <v>513</v>
       </c>
     </row>
     <row r="33">
@@ -14012,7 +14012,7 @@
         <v>182</v>
       </c>
       <c r="J33" t="n">
-        <v>119</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="34">
@@ -14037,7 +14037,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -14473,7 +14473,7 @@
         <v>75</v>
       </c>
       <c r="J19" t="n">
-        <v>60</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
@@ -14498,7 +14498,7 @@
         <v>28</v>
       </c>
       <c r="J20" t="n">
-        <v>22</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21">
@@ -14523,7 +14523,7 @@
         <v>29</v>
       </c>
       <c r="J21" t="n">
-        <v>17</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22">
@@ -14548,7 +14548,7 @@
         <v>29</v>
       </c>
       <c r="J22" t="n">
-        <v>9</v>
+        <v>539</v>
       </c>
     </row>
     <row r="23">
@@ -14573,7 +14573,7 @@
         <v>10</v>
       </c>
       <c r="J23" t="n">
-        <v>29</v>
+        <v>506</v>
       </c>
     </row>
     <row r="24">
@@ -14598,7 +14598,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27">
@@ -14630,7 +14630,7 @@
         <v>202</v>
       </c>
       <c r="J28" t="n">
-        <v>136</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29">
@@ -14655,7 +14655,7 @@
         <v>75</v>
       </c>
       <c r="J29" t="n">
-        <v>51</v>
+        <v>680</v>
       </c>
     </row>
     <row r="30">
@@ -14680,7 +14680,7 @@
         <v>68</v>
       </c>
       <c r="J30" t="n">
-        <v>59</v>
+        <v>871</v>
       </c>
     </row>
     <row r="31">
@@ -14705,7 +14705,7 @@
         <v>69</v>
       </c>
       <c r="J31" t="n">
-        <v>27</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="32">
@@ -14730,7 +14730,7 @@
         <v>28</v>
       </c>
       <c r="J32" t="n">
-        <v>67</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="33">
@@ -14755,7 +14755,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36">
@@ -14823,7 +14823,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3">
@@ -14843,7 +14843,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4">
@@ -14863,7 +14863,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -14883,7 +14883,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6">
@@ -14903,7 +14903,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7">
@@ -14923,7 +14923,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -14943,7 +14943,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -15003,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
@@ -15023,7 +15023,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13">
@@ -15043,7 +15043,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -15063,7 +15063,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15">
@@ -15103,7 +15103,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -15123,7 +15123,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18">
@@ -15143,7 +15143,7 @@
         <v>13</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
@@ -15163,7 +15163,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -15183,7 +15183,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -15203,7 +15203,7 @@
         <v>19</v>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -15223,7 +15223,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -15243,7 +15243,7 @@
         <v>6</v>
       </c>
       <c r="G23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -17449,7 +17449,7 @@
         <v>26.8</v>
       </c>
       <c r="G2" t="n">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -17476,7 +17476,7 @@
         <v>5.33</v>
       </c>
       <c r="G5" t="n">
-        <v>4.92</v>
+        <v>61.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
400 families prune randomly
</commit_message>
<xml_diff>
--- a/outputs-card-100-families-6-games.xlsx
+++ b/outputs-card-100-families-6-games.xlsx
@@ -12881,22 +12881,22 @@
         <v>29</v>
       </c>
       <c r="AI3" t="n">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="AJ3" t="n">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="AK3" t="n">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="AL3" t="n">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="AM3" t="n">
         <v>287</v>
       </c>
       <c r="AN3" t="n">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4">
@@ -12996,22 +12996,22 @@
         <v>69</v>
       </c>
       <c r="AI4" t="n">
-        <v>765</v>
+        <v>777</v>
       </c>
       <c r="AJ4" t="n">
-        <v>799</v>
+        <v>817</v>
       </c>
       <c r="AK4" t="n">
-        <v>779</v>
+        <v>740</v>
       </c>
       <c r="AL4" t="n">
-        <v>817</v>
+        <v>754</v>
       </c>
       <c r="AM4" t="n">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="AN4" t="n">
-        <v>745</v>
+        <v>794</v>
       </c>
     </row>
     <row r="6">
@@ -13111,22 +13111,22 @@
         <v>6</v>
       </c>
       <c r="AI6" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="AK6" t="n">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="AL6" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="AM6" t="n">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="AN6" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -13226,22 +13226,22 @@
         <v>10</v>
       </c>
       <c r="AI7" t="n">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="AJ7" t="n">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="AK7" t="n">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="AL7" t="n">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="AM7" t="n">
-        <v>146</v>
+        <v>77</v>
       </c>
       <c r="AN7" t="n">
-        <v>163</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8">
@@ -13341,22 +13341,22 @@
         <v>10</v>
       </c>
       <c r="AI8" t="n">
+        <v>49</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>75</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>56</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>92</v>
+      </c>
+      <c r="AM8" t="n">
         <v>91</v>
       </c>
-      <c r="AJ8" t="n">
-        <v>120</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>111</v>
-      </c>
-      <c r="AL8" t="n">
-        <v>82</v>
-      </c>
-      <c r="AM8" t="n">
-        <v>49</v>
-      </c>
       <c r="AN8" t="n">
-        <v>45</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9">
@@ -13459,19 +13459,19 @@
         <v>53</v>
       </c>
       <c r="AJ9" t="n">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="AK9" t="n">
+        <v>47</v>
+      </c>
+      <c r="AL9" t="n">
         <v>35</v>
       </c>
-      <c r="AL9" t="n">
-        <v>72</v>
-      </c>
       <c r="AM9" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AN9" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -13571,19 +13571,19 @@
         <v>1</v>
       </c>
       <c r="AI10" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="AJ10" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="AK10" t="n">
+        <v>12</v>
+      </c>
+      <c r="AL10" t="n">
         <v>13</v>
       </c>
-      <c r="AL10" t="n">
-        <v>30</v>
-      </c>
       <c r="AM10" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AN10" t="n">
         <v>15</v>
@@ -13648,7 +13648,7 @@
         <v>29</v>
       </c>
       <c r="J14" t="n">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15">
@@ -13673,7 +13673,7 @@
         <v>74</v>
       </c>
       <c r="J15" t="n">
-        <v>781</v>
+        <v>778</v>
       </c>
     </row>
     <row r="16">
@@ -13723,7 +13723,7 @@
         <v>10</v>
       </c>
       <c r="J17" t="n">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18">
@@ -13748,7 +13748,7 @@
         <v>9</v>
       </c>
       <c r="J18" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19">
@@ -13830,7 +13830,7 @@
         <v>29</v>
       </c>
       <c r="J23" t="n">
-        <v>282</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24">
@@ -13855,7 +13855,7 @@
         <v>71</v>
       </c>
       <c r="J24" t="n">
-        <v>718</v>
+        <v>690</v>
       </c>
     </row>
     <row r="25">
@@ -13880,7 +13880,7 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">
@@ -13987,7 +13987,7 @@
         <v>78</v>
       </c>
       <c r="J32" t="n">
-        <v>516</v>
+        <v>582</v>
       </c>
     </row>
     <row r="33">
@@ -14012,7 +14012,7 @@
         <v>182</v>
       </c>
       <c r="J33" t="n">
-        <v>2084</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="34">
@@ -14037,7 +14037,7 @@
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35">
@@ -14473,7 +14473,7 @@
         <v>75</v>
       </c>
       <c r="J19" t="n">
-        <v>449</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20">
@@ -14498,7 +14498,7 @@
         <v>28</v>
       </c>
       <c r="J20" t="n">
-        <v>333</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21">
@@ -14523,7 +14523,7 @@
         <v>29</v>
       </c>
       <c r="J21" t="n">
-        <v>263</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22">
@@ -14548,7 +14548,7 @@
         <v>29</v>
       </c>
       <c r="J22" t="n">
-        <v>160</v>
+        <v>272</v>
       </c>
     </row>
     <row r="23">
@@ -14573,7 +14573,7 @@
         <v>10</v>
       </c>
       <c r="J23" t="n">
-        <v>293</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24">
@@ -14598,7 +14598,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>220</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
@@ -14630,7 +14630,7 @@
         <v>202</v>
       </c>
       <c r="J28" t="n">
-        <v>1202</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="29">
@@ -14655,7 +14655,7 @@
         <v>75</v>
       </c>
       <c r="J29" t="n">
-        <v>913</v>
+        <v>946</v>
       </c>
     </row>
     <row r="30">
@@ -14680,7 +14680,7 @@
         <v>68</v>
       </c>
       <c r="J30" t="n">
-        <v>729</v>
+        <v>838</v>
       </c>
     </row>
     <row r="31">
@@ -14705,7 +14705,7 @@
         <v>69</v>
       </c>
       <c r="J31" t="n">
-        <v>438</v>
+        <v>753</v>
       </c>
     </row>
     <row r="32">
@@ -14730,7 +14730,7 @@
         <v>28</v>
       </c>
       <c r="J32" t="n">
-        <v>791</v>
+        <v>755</v>
       </c>
     </row>
     <row r="33">
@@ -14755,7 +14755,7 @@
         <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>611</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36">
@@ -14823,7 +14823,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>412</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3">
@@ -14843,7 +14843,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>89</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -14863,7 +14863,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -14883,7 +14883,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>38</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6">
@@ -14903,7 +14903,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7">
@@ -14923,7 +14923,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>61</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8">
@@ -14943,7 +14943,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>123</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -14963,7 +14963,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10">
@@ -14983,7 +14983,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -15003,7 +15003,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -15023,7 +15023,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
@@ -15043,7 +15043,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -15063,7 +15063,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
@@ -15103,7 +15103,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -15123,7 +15123,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>67</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18">
@@ -15163,7 +15163,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
@@ -15203,7 +15203,7 @@
         <v>19</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22">
@@ -15223,7 +15223,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -15263,7 +15263,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -15323,7 +15323,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -15343,7 +15343,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -17449,7 +17449,7 @@
         <v>26.8</v>
       </c>
       <c r="G2" t="n">
-        <v>4.1</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -17476,7 +17476,7 @@
         <v>5.33</v>
       </c>
       <c r="G5" t="n">
-        <v>89.31</v>
+        <v>59.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>